<commit_message>
Updated q in wind tunnel testing
</commit_message>
<xml_diff>
--- a/Wind_Tunnel_Testing/WIND TUNNEL TESTING.xlsx
+++ b/Wind_Tunnel_Testing/WIND TUNNEL TESTING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/G/Programs/GitHub/Sizing_Algorithm/Wind_Tunnel_Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509A4896-A33F-2741-9A04-460C7AB02353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92F29A6-BA6C-154B-8CA4-081FC5A3A783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33680" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{D897026C-7703-4763-9101-B209D1D946C8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" activeTab="2" xr2:uid="{D897026C-7703-4763-9101-B209D1D946C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Scaled Stall Speed" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>CL</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>AOA rel(deg)</t>
+  </si>
+  <si>
+    <t>q A/C (assume sea level)</t>
   </si>
 </sst>
 </file>
@@ -1681,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A213108A-79CB-4518-916B-E4995755C4B6}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1794,12 +1797,12 @@
         <v>0.4723914001721809</v>
       </c>
       <c r="I3">
-        <f>$B$33*$K$1*$N$1*H3</f>
-        <v>41.799030250357511</v>
+        <f>$B$34*$K$1*$N$1*H3</f>
+        <v>5.4628086465078525</v>
       </c>
       <c r="J3">
         <f>I3*0.224809</f>
-        <v>9.3967981915526213</v>
+        <v>1.2280885490127837</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1833,12 +1836,12 @@
         <v>0.53680746580813454</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I3:I30" si="3">$B$33*$K$1*$N$1*H4</f>
-        <v>47.498814529124758</v>
+        <f t="shared" ref="I4:I30" si="3">$B$34*$K$1*$N$1*H4</f>
+        <v>6.2077261877709757</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J30" si="4">I4*0.224809</f>
-        <v>10.678160995478008</v>
+        <v>1.3955527165466053</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1873,11 +1876,11 @@
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>47.611613051580683</v>
+        <v>6.2224680786735824</v>
       </c>
       <c r="J5">
         <f t="shared" si="4"/>
-        <v>10.703519118512801</v>
+        <v>1.3988668262985295</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>10</v>
@@ -1919,18 +1922,18 @@
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>52.182791913862239</v>
+        <v>6.8198856566422021</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>11.731161267363456</v>
+        <v>1.5331716745840769</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="N6" s="4">
         <f>MAX(J:J)</f>
-        <v>17.171825989880507</v>
+        <v>2.2442243021426354</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1965,11 +1968,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>60.120651479120447</v>
+        <v>7.8573022571741413</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>13.515663538369589</v>
+        <v>1.7663922631330615</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -2004,11 +2007,11 @@
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>61.64133584275622</v>
+        <v>8.0560438940140955</v>
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>13.857527069474184</v>
+        <v>1.8110711717694148</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2043,11 +2046,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>61.460164091223163</v>
+        <v>8.0323661530509707</v>
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>13.816798029183788</v>
+        <v>1.8057482025012357</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -2082,11 +2085,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>50.369998237804005</v>
+        <v>6.5829676011612142</v>
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>11.323628933842482</v>
+        <v>1.4799103634494515</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -2121,11 +2124,11 @@
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>48.980741708712486</v>
+        <v>6.4014025616403814</v>
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>11.011311562793946</v>
+        <v>1.4390929084798125</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -2160,11 +2163,11 @@
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>51.544884576517447</v>
+        <v>6.7365161215777336</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>11.587753956762311</v>
+        <v>1.5144294527757687</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -2199,11 +2202,11 @@
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>54.350623228427196</v>
+        <v>7.1032043742881594</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>12.218509257359489</v>
+        <v>1.5968642721793469</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -2238,11 +2241,11 @@
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>52.040818124982202</v>
+        <v>6.8013307849902516</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>11.699244281859125</v>
+        <v>1.5290003724428736</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -2277,11 +2280,11 @@
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>55.790647333520752</v>
+        <v>7.2914043417363885</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>12.542239636401467</v>
+        <v>1.6391733186614159</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -2316,11 +2319,11 @@
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>63.023008565857999</v>
+        <v>8.2366177889871697</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>14.168139532681971</v>
+        <v>1.8516658085244166</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -2355,11 +2358,11 @@
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>62.887444921409397</v>
+        <v>8.2189006734318486</v>
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>14.137663605337126</v>
+        <v>1.8476828414935405</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2394,11 +2397,11 @@
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>62.560409087183359</v>
+        <v>8.1761596296270671</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>14.064143006480604</v>
+        <v>1.8380742701768313</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -2433,11 +2436,11 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>70.464886069234424</v>
+        <v>9.2092133857797354</v>
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>15.841140572338523</v>
+        <v>2.0703140520437566</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -2472,11 +2475,11 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>71.503319662160337</v>
+        <v>9.3449285920006133</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>16.074589789930602</v>
+        <v>2.1008240518390662</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2511,11 +2514,11 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>72.570670196531395</v>
+        <v>9.4844230179022073</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>16.314539796212028</v>
+        <v>2.1321836542315773</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2550,11 +2553,11 @@
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>73.472116121337322</v>
+        <v>9.6022349997327403</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>16.517192953121722</v>
+        <v>2.1586688480549179</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -2589,11 +2592,11 @@
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>76.384068208481452</v>
+        <v>9.9828045235850666</v>
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>17.171825989880507</v>
+        <v>2.2442243021426354</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -2628,11 +2631,11 @@
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>75.864286812737092</v>
+        <v>9.914873131733172</v>
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>17.054974454084615</v>
+        <v>2.2289527138718026</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -2667,11 +2670,11 @@
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>72.589786113860995</v>
+        <v>9.486921319844825</v>
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>16.318837226470976</v>
+        <v>2.1327452949929953</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -2706,11 +2709,11 @@
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>69.455237122631573</v>
+        <v>9.0772601092945138</v>
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>15.614162402301682</v>
+        <v>2.0406497679103905</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -2745,11 +2748,11 @@
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>73.198038191121654</v>
+        <v>9.5664151427161705</v>
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>16.455577767707869</v>
+        <v>2.1506162218188796</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2784,11 +2787,11 @@
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>71.133948643375632</v>
+        <v>9.2966546683449494</v>
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>15.991551860568633</v>
+        <v>2.08997163933596</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -2823,11 +2826,11 @@
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>72.758848808040355</v>
+        <v>9.5090165010495866</v>
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>16.356844041686745</v>
+        <v>2.1377124905844567</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -2862,11 +2865,11 @@
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>71.161862666327309</v>
+        <v>9.3003028143671393</v>
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>15.997827184154376</v>
+        <v>2.0907917753950622</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2876,6 +2879,15 @@
       <c r="B33">
         <f>AVERAGE(E3:E30)</f>
         <v>97.964506372246788</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <f>0.5*1.225*4.572^2</f>
+        <v>12.803200200000001</v>
       </c>
     </row>
   </sheetData>
@@ -2887,10 +2899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E50342-A1ED-3641-9FD6-F5197EE56D46}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3007,12 +3019,12 @@
         <v>0.56366431276522444</v>
       </c>
       <c r="J3">
-        <f>$C$29*$L$1*$O$1*I3</f>
-        <v>49.888341206174275</v>
+        <f>$C$30*$L$1*$O$1*I3</f>
+        <v>8.37239807714686</v>
       </c>
       <c r="K3">
         <f>J3*0.224809</f>
-        <v>11.215348098218833</v>
+        <v>1.8821904393253086</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -3049,12 +3061,12 @@
         <v>0.66835206055644125</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J25" si="4">$C$29*$L$1*$O$1*I4</f>
-        <v>59.153958992570274</v>
+        <f t="shared" ref="J4:J25" si="4">$C$30*$L$1*$O$1*I4</f>
+        <v>9.9273794347711295</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K25" si="5">J4*0.224809</f>
-        <v>13.298342367160732</v>
+        <v>2.2317642433514631</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -3092,11 +3104,11 @@
       </c>
       <c r="J5">
         <f t="shared" si="4"/>
-        <v>58.922178092772853</v>
+        <v>9.8884813292646037</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>13.246235934858174</v>
+        <v>2.2230195991506463</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>10</v>
@@ -3141,18 +3153,18 @@
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>69.005594294151862</v>
+        <v>11.580707857033959</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>15.513078647673987</v>
+        <v>2.6034473526319473</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O6" s="4">
         <f>MAX(K:K)</f>
-        <v>24.459308092529394</v>
+        <v>4.1048280838989166</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -3190,11 +3202,11 @@
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>75.939346452728358</v>
+        <v>12.744349137467914</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>17.071848536691409</v>
+        <v>2.8650443852450245</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -3232,11 +3244,11 @@
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>82.451144664325184</v>
+        <v>13.837176950688416</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>18.535759380842283</v>
+        <v>3.1107219131073123</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3274,11 +3286,11 @@
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>78.827657125085196</v>
+        <v>13.229073346266631</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>17.721166770633278</v>
+        <v>2.9740147499008551</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3316,11 +3328,11 @@
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>82.19079508005079</v>
+        <v>13.793484370296603</v>
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>18.47723045115114</v>
+        <v>3.1008994278020094</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -3358,11 +3370,11 @@
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>85.646599510499669</v>
+        <v>14.373446936077503</v>
       </c>
       <c r="K11">
         <f t="shared" si="5"/>
-        <v>19.254126389355921</v>
+        <v>3.2312802322526477</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -3400,11 +3412,11 @@
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>73.684222255463368</v>
+        <v>12.365888017366128</v>
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>16.564876321028464</v>
+        <v>2.7799629192960622</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -3442,11 +3454,11 @@
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>81.979319088687731</v>
+        <v>13.757993890143462</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>18.4296887450088</v>
+        <v>3.0929208484492619</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -3484,11 +3496,11 @@
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>82.527437159828878</v>
+        <v>13.849980566266975</v>
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>18.552910620463972</v>
+        <v>3.1136002811219123</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -3526,11 +3538,11 @@
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>84.826788427969618</v>
+        <v>14.235863994551501</v>
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>19.069825479703422</v>
+        <v>3.2003503487511287</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -3568,11 +3580,11 @@
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>92.757768352047037</v>
+        <v>15.566862770233749</v>
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>20.852781145455342</v>
+        <v>3.4995708525134792</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -3610,11 +3622,11 @@
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>92.584171457889994</v>
+        <v>15.537729263933498</v>
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>20.813755001276792</v>
+        <v>3.4930213780956261</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -3652,11 +3664,11 @@
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>99.33103761010851</v>
+        <v>16.670006822855633</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>22.330511234090885</v>
+        <v>3.7475675638393522</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -3694,11 +3706,11 @@
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>102.53447306389161</v>
+        <v>17.207616135674364</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>23.05067235502041</v>
+        <v>3.8684269758448182</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -3736,11 +3748,11 @@
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>108.8003954135706</v>
+        <v>18.259180388235865</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>24.459308092529394</v>
+        <v>4.1048280838989166</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -3778,11 +3790,11 @@
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>106.81413709488757</v>
+        <v>17.925841076364726</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>24.012779346164582</v>
+        <v>4.0298904065364782</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -3820,11 +3832,11 @@
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>104.24678695186454</v>
+        <v>17.494981342785362</v>
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>23.435615927861715</v>
+        <v>3.9330292606902346</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3862,11 +3874,11 @@
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>106.18216064179025</v>
+        <v>17.819781056873452</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>23.870705351720225</v>
+        <v>4.0060471596146643</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -3904,11 +3916,11 @@
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>104.930014968413</v>
+        <v>17.609642540045119</v>
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>23.58921173503396</v>
+        <v>3.9588061297850032</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -3946,11 +3958,11 @@
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>98.632395757068721</v>
+        <v>16.552758833333769</v>
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>22.173450257750861</v>
+        <v>3.7212091605629314</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -3960,6 +3972,15 @@
       <c r="C29">
         <f>AVERAGE(F3:F25)</f>
         <v>97.990292870269784</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <f>0.5*1.225*5.1816^2</f>
+        <v>16.444999368000005</v>
       </c>
     </row>
   </sheetData>
@@ -3970,10 +3991,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E545F03-1D0D-2D47-BB11-364EDC77AB76}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4090,12 +4111,12 @@
         <v>0.40580082444362725</v>
       </c>
       <c r="J3">
-        <f>$C$35*$L$1*$O$1*I3</f>
-        <v>62.800766960728829</v>
+        <f>$C$36*$L$1*$O$1*I3</f>
+        <v>8.3426572935452796</v>
       </c>
       <c r="K3">
         <f>J3*0.224809</f>
-        <v>14.118177619674489</v>
+        <v>1.8755044435046209</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -4132,12 +4153,12 @@
         <v>0.4210865004699908</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J32" si="4">$C$35*$L$1*$O$1*I4</f>
-        <v>65.166341696277968</v>
+        <f t="shared" ref="J4:J32" si="4">$C$36*$L$1*$O$1*I4</f>
+        <v>8.6569079034669141</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K32" si="5">J4*0.224809</f>
-        <v>14.649980110398554</v>
+        <v>1.9461508088704935</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -4175,11 +4196,11 @@
       </c>
       <c r="J5">
         <f t="shared" si="4"/>
-        <v>73.69583353347835</v>
+        <v>9.7899932259814015</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>16.567486640827735</v>
+        <v>2.2008785871396528</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>10</v>
@@ -4224,18 +4245,18 @@
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>84.283704666656078</v>
+        <v>11.196520321224661</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>18.947735362406288</v>
+        <v>2.517078536894195</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O6" s="4">
         <f>MAX(K:K)</f>
-        <v>34.427621924560498</v>
+        <v>4.5734768068670197</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -4273,11 +4294,11 @@
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>98.951275653736019</v>
+        <v>13.145007959130023</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>22.245137328440741</v>
+        <v>2.9551160942840613</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -4315,11 +4336,11 @@
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>90.647833499574205</v>
+        <v>12.041951808680974</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>20.378448801205778</v>
+        <v>2.707139144157761</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -4357,11 +4378,11 @@
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>98.490690580709824</v>
+        <v>13.083822346202988</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>22.141593658758797</v>
+        <v>2.9413610178275476</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -4399,11 +4420,11 @@
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>104.20890342428474</v>
+        <v>13.843448261525422</v>
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>23.427099369910028</v>
+        <v>3.1121317602252687</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -4441,11 +4462,11 @@
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>108.01718302618752</v>
+        <v>14.349352458786921</v>
       </c>
       <c r="K11">
         <f t="shared" si="5"/>
-        <v>24.283234898934193</v>
+        <v>3.2258635769074289</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -4483,11 +4504,11 @@
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>102.18972195950447</v>
+        <v>13.575213655653897</v>
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>22.973169203994242</v>
+        <v>3.0518302067138969</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -4525,11 +4546,11 @@
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>104.89811833320199</v>
+        <v>13.935005802379887</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>23.582041084368807</v>
+        <v>3.13271471942722</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -4567,11 +4588,11 @@
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>114.51062800512004</v>
+        <v>15.211962721932307</v>
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>25.743019771203031</v>
+        <v>3.4197861275548802</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -4609,11 +4630,11 @@
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>115.42238376915722</v>
+        <v>15.333083310786472</v>
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>25.947990672760469</v>
+        <v>3.447015126014596</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -4651,11 +4672,11 @@
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>116.97554591065413</v>
+        <v>15.539410400325368</v>
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>26.297155500628246</v>
+        <v>3.4933993126867455</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -4693,11 +4714,11 @@
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>124.63776299254479</v>
+        <v>16.557284135258183</v>
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>28.019690860591005</v>
+        <v>3.722226489163257</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -4735,11 +4756,11 @@
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>123.56779884686907</v>
+        <v>16.415146632553235</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>27.779153290965787</v>
+        <v>3.6902726993176604</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -4777,11 +4798,11 @@
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>130.44153734122543</v>
+        <v>17.328276318050936</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>29.324431568143549</v>
+        <v>3.8955524707847129</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -4819,11 +4840,11 @@
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>134.50381959336738</v>
+        <v>17.867923050079931</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>30.23766917896533</v>
+        <v>4.0168699129654195</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -4861,11 +4882,11 @@
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>138.68572610981127</v>
+        <v>18.423461056839496</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>31.177799401020565</v>
+        <v>4.1417598567270302</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -4903,11 +4924,11 @@
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>150.64684907961563</v>
+        <v>20.012415373996646</v>
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>33.866767494739314</v>
+        <v>4.4989710878128122</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -4945,11 +4966,11 @@
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>147.06318709904747</v>
+        <v>19.536350109085415</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>33.061128028549767</v>
+        <v>4.391947331673383</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -4987,11 +5008,11 @@
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>148.58888840213675</v>
+        <v>19.739029211905113</v>
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>33.404119412795964</v>
+        <v>4.4375114180991764</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -5029,11 +5050,11 @@
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>153.14165324591318</v>
+        <v>20.343833240070548</v>
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>34.427621924560498</v>
+        <v>4.5734768068670197</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -5071,11 +5092,11 @@
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>152.87534716030265</v>
+        <v>20.308456277097736</v>
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>34.367753919760482</v>
+        <v>4.565523747198065</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -5113,11 +5134,11 @@
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>145.02985860804665</v>
+        <v>19.266236166428804</v>
       </c>
       <c r="K27">
         <f t="shared" si="5"/>
-        <v>32.604017483816364</v>
+        <v>4.3312232863386928</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -5155,11 +5176,11 @@
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>144.33069657255692</v>
+        <v>19.173357217061898</v>
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>32.446839565779946</v>
+        <v>4.3103432626104681</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -5197,11 +5218,11 @@
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>144.95326804496912</v>
+        <v>19.256061627954217</v>
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>32.586799235921461</v>
+        <v>4.3289359585187599</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -5239,11 +5260,11 @@
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>146.0357210499285</v>
+        <v>19.399858191177586</v>
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>32.830144413513374</v>
+        <v>4.3612627201004424</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -5281,11 +5302,11 @@
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
-        <v>150.93917288727536</v>
+        <v>20.05124861543738</v>
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>33.932484517615485</v>
+        <v>4.5077011499878621</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -5323,11 +5344,11 @@
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
-        <v>147.17444048538803</v>
+        <v>19.551129369274481</v>
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>33.086138791079598</v>
+        <v>4.3952698423772265</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
@@ -5337,6 +5358,15 @@
       <c r="C35">
         <f>AVERAGE(F3:F32)</f>
         <v>171.33912854443238</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <f>0.5*1.225*6.096^2</f>
+        <v>22.761244800000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>